<commit_message>
Some changes in the test cases
</commit_message>
<xml_diff>
--- a/Test-Cases/Test_Cases_nopCommerce.xlsx
+++ b/Test-Cases/Test_Cases_nopCommerce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Desktop\Ecommerce-Manual-Testing\Test-Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81FC30DB-9B37-490D-B644-BA35AB1DBF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{619F1338-CE24-445F-B403-35CF3D33627A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1065,7 +1065,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+      <selection pane="bottomLeft" activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>